<commit_message>
Database Attempt 1 Upload
</commit_message>
<xml_diff>
--- a/Excel Documents/Database_Plan.xlsx
+++ b/Excel Documents/Database_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CONS\Desktop\coursework Software design and analysis\Database_Design_Git\Excel Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF86D3-D920-4A0A-8A89-77C307F7C40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149AB3BA-9A03-4535-973E-8C8EE8306906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="16404" windowHeight="10500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7380" windowHeight="14400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Cases" sheetId="7" r:id="rId1"/>
@@ -5160,7 +5160,7 @@
   </sheetPr>
   <dimension ref="A1:AC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H73" zoomScale="56" zoomScaleNormal="38" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>

</xml_diff>